<commit_message>
update ratings employee model
</commit_message>
<xml_diff>
--- a/Examples/AHP_Ratings_Employee_Evaluation/Ratings_Employee_Eval_criteriapriorities.xlsx
+++ b/Examples/AHP_Ratings_Employee_Evaluation/Ratings_Employee_Eval_criteriapriorities.xlsx
@@ -732,10 +732,10 @@
       <c r="I4" s="18" t="n"/>
       <c r="J4" s="18" t="n"/>
       <c r="K4" s="17" t="n">
-        <v>0.064</v>
+        <v>0.077</v>
       </c>
       <c r="L4" s="17" t="n">
-        <v>0.255</v>
+        <v>0.213</v>
       </c>
     </row>
     <row r="5">
@@ -766,10 +766,10 @@
       <c r="I5" s="18" t="n"/>
       <c r="J5" s="18" t="n"/>
       <c r="K5" s="17" t="n">
-        <v>0.207</v>
+        <v>0.193</v>
       </c>
       <c r="L5" s="17" t="n">
-        <v>0.819</v>
+        <v>0.531</v>
       </c>
     </row>
     <row r="6">
@@ -800,10 +800,10 @@
       <c r="I6" s="18" t="n"/>
       <c r="J6" s="18" t="n"/>
       <c r="K6" s="17" t="n">
-        <v>0.044</v>
+        <v>0.049</v>
       </c>
       <c r="L6" s="17" t="n">
-        <v>0.174</v>
+        <v>0.135</v>
       </c>
     </row>
     <row r="7">
@@ -824,8 +824,8 @@
       <c r="E7" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="8" t="n">
-        <v>0.25</v>
+      <c r="F7" s="7" t="n">
+        <v>4</v>
       </c>
       <c r="G7" s="8" t="n">
         <v>3</v>
@@ -834,7 +834,7 @@
       <c r="I7" s="18" t="n"/>
       <c r="J7" s="18" t="n"/>
       <c r="K7" s="17" t="n">
-        <v>0.253</v>
+        <v>0.363</v>
       </c>
       <c r="L7" s="17" t="n">
         <v>1</v>
@@ -856,7 +856,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="11" t="n">
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="F8" s="6" t="n">
         <v>1</v>
@@ -868,10 +868,10 @@
       <c r="I8" s="18" t="n"/>
       <c r="J8" s="18" t="n"/>
       <c r="K8" s="17" t="n">
-        <v>0.197</v>
+        <v>0.083</v>
       </c>
       <c r="L8" s="17" t="n">
-        <v>0.779</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="9">
@@ -905,7 +905,7 @@
         <v>0.235</v>
       </c>
       <c r="L9" s="17" t="n">
-        <v>0.929</v>
+        <v>0.649</v>
       </c>
     </row>
     <row r="10">
@@ -946,7 +946,7 @@
         </is>
       </c>
       <c r="L10" s="21" t="n">
-        <v>0.304</v>
+        <v>0.102</v>
       </c>
     </row>
     <row r="11">
@@ -1320,7 +1320,7 @@
         </is>
       </c>
       <c r="C4" s="8" t="n">
-        <v>0.064</v>
+        <v>0.077</v>
       </c>
       <c r="D4" s="8" t="n">
         <v>0</v>
@@ -1370,7 +1370,7 @@
         </is>
       </c>
       <c r="C5" s="8" t="n">
-        <v>0.207</v>
+        <v>0.193</v>
       </c>
       <c r="D5" s="8" t="n">
         <v>0</v>
@@ -1420,7 +1420,7 @@
         </is>
       </c>
       <c r="C6" s="8" t="n">
-        <v>0.044</v>
+        <v>0.049</v>
       </c>
       <c r="D6" s="8" t="n">
         <v>0</v>
@@ -1470,7 +1470,7 @@
         </is>
       </c>
       <c r="C7" s="8" t="n">
-        <v>0.253</v>
+        <v>0.363</v>
       </c>
       <c r="D7" s="8" t="n">
         <v>0</v>
@@ -1520,7 +1520,7 @@
         </is>
       </c>
       <c r="C8" s="8" t="n">
-        <v>0.197</v>
+        <v>0.083</v>
       </c>
       <c r="D8" s="8" t="n">
         <v>0</v>
@@ -2177,7 +2177,7 @@
         </is>
       </c>
       <c r="C4" s="8" t="n">
-        <v>0.054</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D4" s="8" t="n">
         <v>0</v>
@@ -2227,7 +2227,7 @@
         </is>
       </c>
       <c r="C5" s="8" t="n">
-        <v>0.173</v>
+        <v>0.178</v>
       </c>
       <c r="D5" s="8" t="n">
         <v>0</v>
@@ -2277,7 +2277,7 @@
         </is>
       </c>
       <c r="C6" s="8" t="n">
-        <v>0.037</v>
+        <v>0.045</v>
       </c>
       <c r="D6" s="8" t="n">
         <v>0</v>
@@ -2327,7 +2327,7 @@
         </is>
       </c>
       <c r="C7" s="8" t="n">
-        <v>0.211</v>
+        <v>0.335</v>
       </c>
       <c r="D7" s="8" t="n">
         <v>0</v>
@@ -2377,7 +2377,7 @@
         </is>
       </c>
       <c r="C8" s="8" t="n">
-        <v>0.165</v>
+        <v>0.077</v>
       </c>
       <c r="D8" s="8" t="n">
         <v>0</v>
@@ -2427,7 +2427,7 @@
         </is>
       </c>
       <c r="C9" s="8" t="n">
-        <v>0.196</v>
+        <v>0.217</v>
       </c>
       <c r="D9" s="8" t="n">
         <v>0</v>
@@ -2481,7 +2481,7 @@
         </is>
       </c>
       <c r="C10" s="8" t="n">
-        <v>0.1</v>
+        <v>0.047</v>
       </c>
       <c r="D10" s="8" t="n">
         <v>0</v>
@@ -2531,7 +2531,7 @@
         </is>
       </c>
       <c r="C11" s="8" t="n">
-        <v>0.064</v>
+        <v>0.03</v>
       </c>
       <c r="D11" s="8" t="n">
         <v>0</v>
@@ -2885,7 +2885,7 @@
         </is>
       </c>
       <c r="C3" s="8" t="n">
-        <v>0.054</v>
+        <v>0.07099999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -2896,7 +2896,7 @@
         </is>
       </c>
       <c r="C4" s="8" t="n">
-        <v>0.173</v>
+        <v>0.178</v>
       </c>
     </row>
     <row r="5">
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="C5" s="8" t="n">
-        <v>0.037</v>
+        <v>0.045</v>
       </c>
     </row>
     <row r="6">
@@ -2918,7 +2918,7 @@
         </is>
       </c>
       <c r="C6" s="8" t="n">
-        <v>0.211</v>
+        <v>0.335</v>
       </c>
     </row>
     <row r="7">
@@ -2929,7 +2929,7 @@
         </is>
       </c>
       <c r="C7" s="8" t="n">
-        <v>0.165</v>
+        <v>0.077</v>
       </c>
     </row>
     <row r="8">
@@ -2940,7 +2940,7 @@
         </is>
       </c>
       <c r="C8" s="8" t="n">
-        <v>0.196</v>
+        <v>0.217</v>
       </c>
     </row>
     <row r="9">
@@ -2955,7 +2955,7 @@
         </is>
       </c>
       <c r="C9" s="8" t="n">
-        <v>0.1</v>
+        <v>0.047</v>
       </c>
     </row>
     <row r="10">
@@ -2966,7 +2966,7 @@
         </is>
       </c>
       <c r="C10" s="8" t="n">
-        <v>0.064</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="11">
@@ -3086,7 +3086,7 @@
         </is>
       </c>
       <c r="C3" s="8" t="n">
-        <v>0.064</v>
+        <v>0.077</v>
       </c>
     </row>
     <row r="4">
@@ -3097,7 +3097,7 @@
         </is>
       </c>
       <c r="C4" s="8" t="n">
-        <v>0.207</v>
+        <v>0.193</v>
       </c>
     </row>
     <row r="5">
@@ -3108,7 +3108,7 @@
         </is>
       </c>
       <c r="C5" s="8" t="n">
-        <v>0.044</v>
+        <v>0.049</v>
       </c>
     </row>
     <row r="6">
@@ -3119,7 +3119,7 @@
         </is>
       </c>
       <c r="C6" s="8" t="n">
-        <v>0.253</v>
+        <v>0.363</v>
       </c>
     </row>
     <row r="7">
@@ -3130,7 +3130,7 @@
         </is>
       </c>
       <c r="C7" s="8" t="n">
-        <v>0.197</v>
+        <v>0.083</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
update Employee evaluation rating model
</commit_message>
<xml_diff>
--- a/Examples/AHP_Ratings_Employee_Evaluation/Ratings_Employee_Eval_criteriapriorities.xlsx
+++ b/Examples/AHP_Ratings_Employee_Evaluation/Ratings_Employee_Eval_criteriapriorities.xlsx
@@ -13,6 +13,8 @@
     <sheet name="limit matrix" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="limitingPriorities" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="localPriorities" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Graph Model1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Graph Model2" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -302,6 +304,72 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="12963525" cy="2790825"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="12963525" cy="2790825"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1085,9 +1153,37 @@
         <color rgb="ff0b30b5"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="3">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="5">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:H16">
     <cfRule type="dataBar" priority="1">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="3">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="5">
       <dataBar showValue="1">
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -3233,4 +3329,42 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>